<commit_message>
Update benchmark data files for English and Chinese documentation
</commit_message>
<xml_diff>
--- a/docs/en/source/_static/ros2_common_benchmark_data.xlsx
+++ b/docs/en/source/_static/ros2_common_benchmark_data.xlsx
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>使用默认launch文件，运行 common_benchmark_node 节点 1h 数据</v>
+        <v>Using the default launch file, run the common_benchmark_node node for 1 hour of data</v>
       </c>
     </row>
     <row r="2">
@@ -1095,16 +1095,16 @@
         <v>37.63</v>
       </c>
       <c r="H9" t="str">
-        <v>73.12</v>
+        <v>108.58</v>
       </c>
       <c r="I9" t="str">
-        <v>55.12</v>
+        <v>98.72</v>
       </c>
       <c r="J9" t="str">
-        <v>0</v>
+        <v>30.06</v>
       </c>
       <c r="K9" t="str">
-        <v>378.99</v>
+        <v/>
       </c>
       <c r="L9" t="str">
         <v>29.94</v>
@@ -1119,16 +1119,16 @@
         <v>37.62</v>
       </c>
       <c r="P9" t="str">
-        <v>66.2</v>
+        <v>114.4</v>
       </c>
       <c r="Q9" t="str">
-        <v>42.5</v>
+        <v>79.88</v>
       </c>
       <c r="R9" t="str">
-        <v>0.07</v>
+        <v>29.73</v>
       </c>
       <c r="S9" t="str">
-        <v>148.47</v>
+        <v>155.01</v>
       </c>
       <c r="T9" t="str">
         <v>3.74</v>

</xml_diff>